<commit_message>
berekning groote schaal model
</commit_message>
<xml_diff>
--- a/Opleverset/Extra documenten/aangepast met berkenign grote tank Scriptie Jelle Willemen-Floating Farm - Bijlage Rekenmodel gewichtsverdeling.xlsx
+++ b/Opleverset/Extra documenten/aangepast met berkenign grote tank Scriptie Jelle Willemen-Floating Farm - Bijlage Rekenmodel gewichtsverdeling.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyril\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyril\Desktop\Project-5-6---Floating-Farm\Opleverset\Extra documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEBD48AD-B7C5-4659-A165-57A84E66DF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E8CC6E-F0B9-49EA-9BFC-C28F1FDF49D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="747" firstSheet="3" activeTab="6" xr2:uid="{C9B0FE52-629E-47BA-9955-0395F0E7E877}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="747" firstSheet="2" activeTab="7" xr2:uid="{C9B0FE52-629E-47BA-9955-0395F0E7E877}"/>
   </bookViews>
   <sheets>
     <sheet name="Toelichting model" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Belastingsverdeling" sheetId="5" r:id="rId5"/>
     <sheet name="Moment verdeling hor. as" sheetId="6" r:id="rId6"/>
     <sheet name="Moment verdeling vert. as" sheetId="7" r:id="rId7"/>
+    <sheet name="groote schaal model" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="584" uniqueCount="226">
   <si>
     <t>Deze rekensheet is een overzicht van de gewichtverdeling van de gehele boerderij</t>
   </si>
@@ -775,15 +776,53 @@
   <si>
     <t>Moment abs (Nm)</t>
   </si>
+  <si>
+    <t>breed</t>
+  </si>
+  <si>
+    <t>lengthe</t>
+  </si>
+  <si>
+    <t>formaat beton blok</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hoogte </t>
+  </si>
+  <si>
+    <t>grote floating farm (m)</t>
+  </si>
+  <si>
+    <t>grote schaal model (cm)</t>
+  </si>
+  <si>
+    <t>volume</t>
+  </si>
+  <si>
+    <t>grote floating farm (cm)</t>
+  </si>
+  <si>
+    <t>ration</t>
+  </si>
+  <si>
+    <t>drijf tank volume</t>
+  </si>
+  <si>
+    <t>m^3</t>
+  </si>
+  <si>
+    <t>cm^3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="1">
-    <numFmt numFmtId="172" formatCode="#,##0.00000"/>
+  <numFmts count="3">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="#,##0.00000"/>
+    <numFmt numFmtId="170" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -821,6 +860,13 @@
     <font>
       <sz val="11"/>
       <color theme="9"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1203,10 +1249,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -1334,12 +1381,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="172" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1682,7 +1732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B67E5702-5F98-4EF8-A149-15FB2E56B1EA}">
   <dimension ref="A1:A17"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="134" workbookViewId="0">
+    <sheetView zoomScale="134" workbookViewId="0">
       <selection activeCell="L28" sqref="L28"/>
     </sheetView>
   </sheetViews>
@@ -1767,8 +1817,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFD6690-25F0-4599-9992-736BE7C8D663}">
   <dimension ref="A1:O56"/>
   <sheetViews>
-    <sheetView topLeftCell="AU16" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2824,7 +2874,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ACF56697-13B9-4E3E-B1DF-4D844660A877}">
   <dimension ref="A1:O53"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
@@ -4159,8 +4209,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{554313C8-6C97-4793-B84F-AC68D80FEE31}">
   <dimension ref="A1:O52"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5443,8 +5493,8 @@
   </sheetPr>
   <dimension ref="A1:AF12"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P8" sqref="P8"/>
+    <sheetView topLeftCell="R1" zoomScale="90" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P7" sqref="P7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6446,7 +6496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{221C7ABC-5C4D-45CF-B17C-4450D6AC5256}">
   <dimension ref="A1:AX60"/>
   <sheetViews>
-    <sheetView topLeftCell="AN7" zoomScale="131" workbookViewId="0">
+    <sheetView topLeftCell="AJ9" zoomScale="91" workbookViewId="0">
       <selection activeCell="AY53" sqref="AY53"/>
     </sheetView>
   </sheetViews>
@@ -7832,7 +7882,7 @@
         <v>1860432.5959570312</v>
       </c>
       <c r="AT15" s="13">
-        <f t="shared" ref="AT15:AT60" si="1">ABS(AR$16)</f>
+        <f t="shared" ref="AT15:AT43" si="1">ABS(AR$16)</f>
         <v>482002.46679721895</v>
       </c>
       <c r="AU15">
@@ -7846,7 +7896,7 @@
         <v>9.81</v>
       </c>
       <c r="AX15">
-        <f t="shared" ref="AX15:AX60" si="2">AT15/(AW15*AV15*AU15)</f>
+        <f t="shared" ref="AX15:AX43" si="2">AT15/(AW15*AV15*AU15)</f>
         <v>24.640816782519781</v>
       </c>
     </row>
@@ -7867,7 +7917,7 @@
         <v>482002.46679721895</v>
       </c>
       <c r="AU16">
-        <f t="shared" ref="AU16:AU60" si="3">AU15+1</f>
+        <f t="shared" ref="AU16:AU43" si="3">AU15+1</f>
         <v>3</v>
       </c>
       <c r="AV16">
@@ -8554,8 +8604,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD6A58AD-E082-4AE4-BE32-52B2B8CD07A6}">
   <dimension ref="A1:AW43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AH7" zoomScale="108" zoomScaleNormal="107" workbookViewId="0">
-      <selection activeCell="AW32" sqref="AW32"/>
+    <sheetView topLeftCell="AP29" zoomScale="146" zoomScaleNormal="107" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10620,13 +10670,141 @@
 </worksheet>
 </file>
 
-<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9D3020A-0241-451B-89B2-1C903AEFDCDE}">
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F3" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4">
+        <v>6.4</v>
+      </c>
+      <c r="C4">
+        <v>5.2</v>
+      </c>
+      <c r="D4">
+        <f>C4*100</f>
+        <v>520</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B5">
+        <v>30</v>
+      </c>
+      <c r="C5">
+        <v>30</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:D6" si="0">C5*100</f>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>215</v>
+      </c>
+      <c r="B6">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>30</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C7" t="s">
+        <v>224</v>
+      </c>
+      <c r="D7" t="s">
+        <v>225</v>
+      </c>
+      <c r="F7" s="56">
+        <f>D8/B8</f>
+        <v>812500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B8">
+        <f>B4*B5*B6</f>
+        <v>5760</v>
+      </c>
+      <c r="C8">
+        <f>C4*C5*C6</f>
+        <v>4680</v>
+      </c>
+      <c r="D8" s="55">
+        <f>D4*D5*D6</f>
+        <v>4680000000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>223</v>
+      </c>
+      <c r="B9">
+        <f>D9/F7</f>
+        <v>11.076923076923077</v>
+      </c>
+      <c r="C9" s="55">
+        <v>9</v>
+      </c>
+      <c r="D9" s="56">
+        <f>C9*1000000</f>
+        <v>9000000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101004CEF96245D7C1E4BABEEA03D7ECE19C0" ma:contentTypeVersion="4" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="f72c6b3f2ff96562f14ae8449ff33f0d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="0714667c-0a60-4810-ab6f-84607c76cfd4" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f69e43b74bb03b9c993e12ef8729ea88" ns2:_="">
     <xsd:import namespace="0714667c-0a60-4810-ab6f-84607c76cfd4"/>
@@ -10770,6 +10948,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -10780,15 +10964,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A23B4FB9-F351-4206-B0AD-FF7C8B58859B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{340E62E5-999B-4585-922A-359AE6FF5DF0}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10806,6 +10981,15 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A23B4FB9-F351-4206-B0AD-FF7C8B58859B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49A34E54-66C2-4D18-8E75-6202DF656FAF}">
   <ds:schemaRefs>

</xml_diff>